<commit_message>
se agregaron los minutos para ahcer las tareas
</commit_message>
<xml_diff>
--- a/static/plantilla_tareas.xlsx
+++ b/static/plantilla_tareas.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tareas" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrucciones" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plantilla Tareas" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,13 +29,6 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
-    <font>
-      <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <i val="1"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -47,12 +39,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="002563eb"/>
-        <bgColor rgb="002563eb"/>
+        <fgColor rgb="000077BE"/>
+        <bgColor rgb="000077BE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -60,24 +52,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -443,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,11 +433,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="45" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -490,236 +473,56 @@
           <t>Etiquetas</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tiempo (min)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Revisar expediente 1234</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Verificar documentacion completa del caso</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ejemplo de tarea</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Descripcion de la tarea</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>2024-12-20</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-01-15</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Urgente, Legal</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Preparar informe mensual</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Elaborar informe de actividades del mes</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Media</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>2024-12-15</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>Administrativo</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Audiencia caso Smith</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Preparar alegatos para audiencia</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Urgente</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>2024-12-10</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>Legal, Importante, Tribunal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="75" customWidth="1" min="1" max="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>INSTRUCCIONES PARA IMPORTAR TAREAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1. Complete la hoja "Tareas" con los datos de las tareas a importar.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2. Columnas requeridas:</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Titulo: Nombre de la tarea (obligatorio)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Descripcion: Detalle de la tarea (opcional)</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Prioridad: Normal, Media o Urgente (obligatorio)</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Fecha Vencimiento: Formato AAAA-MM-DD, ej: 2024-12-20 (obligatorio)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Asignados: Username(s) separados por coma, ej: admin, usuario1 (obligatorio)</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Etiquetas: Nombre(s) de etiquetas separadas por coma (opcional)</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>3. Importante:</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - No modifique los encabezados de las columnas</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Los usernames deben existir en el sistema</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Las etiquetas deben existir en el sistema (se ignoran las que no existan)</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - La fecha debe estar en formato AAAA-MM-DD</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">   - Las prioridades validas son: Normal, Media, Urgente</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Backend, Diseño</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego el excel para mandar quien carga la tarea
</commit_message>
<xml_diff>
--- a/static/plantilla_tareas.xlsx
+++ b/static/plantilla_tareas.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plantilla Tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrucciones" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,6 +30,13 @@
       <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <i val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -39,12 +47,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000077BE"/>
-        <bgColor rgb="000077BE"/>
+        <fgColor rgb="002563eb"/>
+        <bgColor rgb="002563eb"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -52,13 +60,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -424,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,13 +452,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="45" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="18" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="12" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -483,46 +503,308 @@
           <t>Estado</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Completado Por</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Ejemplo de tarea</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Descripcion de la tarea</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Revisar expediente 1234</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Verificar documentacion completa del caso</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-01-15</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-20</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>admin</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Backend, Diseño</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Urgente, Legal</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr"/>
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Preparar informe mensual</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Elaborar informe de actividades del mes</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Media</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-15</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Administrativo</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Completada</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>giuliana</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Audiencia caso Smith</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Preparar alegatos para audiencia</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Urgente</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-10</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>admin, giuliana</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Legal, Tribunal</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>Completada</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="75" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>INSTRUCCIONES PARA IMPORTAR TAREAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1. Complete la hoja "Tareas" con los datos de las tareas a importar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2. Columnas obligatorias:</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Titulo: Nombre de la tarea</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Prioridad: Normal, Media o Urgente</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Fecha Vencimiento: Formato AAAA-MM-DD, ej: 2024-12-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Asignados: Username(s) separados por coma, ej: admin, usuario1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3. Columnas opcionales:</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Descripcion: Detalle de la tarea</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Etiquetas: Nombre(s) de etiquetas separadas por coma</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Tiempo (min): Tiempo dedicado en minutos, ej: 60, 120</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Estado: Pendiente o Completada (por defecto: Pendiente)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Completado Por: Username del usuario que completo la tarea</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     * Si el estado es Completada y no se indica usuario, se usa quien sube el archivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">     * Si el estado es Pendiente, este campo se ignora</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>4. Importante:</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - No modifique los encabezados de las columnas</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Los usernames deben existir en el sistema</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - Las etiquetas deben existir en el sistema (se ignoran las que no existan)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   - La fecha debe estar en formato AAAA-MM-DD</t>
         </is>
       </c>
     </row>

</xml_diff>